<commit_message>
added some lines in the file rd fitness
</commit_message>
<xml_diff>
--- a/RD_Fitness.xlsx
+++ b/RD_Fitness.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perumal.natarajan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perumal.natarajan\Downloads\git_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99DA57AB-16E1-4666-81D6-36B51B6BF4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984C363C-F781-46B2-9D9C-3E40701A60B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{8948C491-46B0-49D1-AE8B-A68E3AA7F592}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>S.No</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Daily 12000 steps</t>
+  </si>
+  <si>
+    <t>Test_commit_in_git</t>
   </si>
 </sst>
 </file>
@@ -79,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -106,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +132,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -143,9 +157,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB4E860-0E8C-4955-85EE-6DB8E8877F52}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -856,6 +874,14 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
     </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>